<commit_message>
Updated SBC1802 BOM spreadsheet and PDF
</commit_message>
<xml_diff>
--- a/hw/SBC1802 BOM.xlsx
+++ b/hw/SBC1802 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fours\Documents\SBC1802\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fours\Git\SBC1802\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CFAAA5-F464-4515-BA1F-8295F839ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA714AC-C0F6-4F9C-9C28-0F5DD50A1606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="270" windowWidth="17930" windowHeight="10530" xr2:uid="{E6317DB6-1395-40AB-B574-B66DE8210E28}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="17910" windowHeight="10170" xr2:uid="{E6317DB6-1395-40AB-B574-B66DE8210E28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="358">
   <si>
     <t>Qty</t>
   </si>
@@ -313,18 +313,9 @@
     <t>U22</t>
   </si>
   <si>
-    <t>Abracon</t>
-  </si>
-  <si>
-    <t>ACH-32.768MHZ-EK</t>
-  </si>
-  <si>
     <t>32768Hz</t>
   </si>
   <si>
-    <t>535-9178-5-ND</t>
-  </si>
-  <si>
     <t>U18,U19,U20,U23</t>
   </si>
   <si>
@@ -442,9 +433,6 @@
     <t>CF18JT4K70CT-ND</t>
   </si>
   <si>
-    <t>R2,R3,R6,R7,R8,R12</t>
-  </si>
-  <si>
     <t>10M Ohms</t>
   </si>
   <si>
@@ -1094,6 +1082,33 @@
   </si>
   <si>
     <t>8 Position Dip Switch, SPST, DIP-16</t>
+  </si>
+  <si>
+    <t>R2,R3,R6,R7,R8,R9,R12</t>
+  </si>
+  <si>
+    <t>Pletronics</t>
+  </si>
+  <si>
+    <t>P1145-HCM-32.768K</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Fuse, 5A</t>
+  </si>
+  <si>
+    <t>FUSE BRD MNT 5A 125VAC/VDC AXIAL</t>
+  </si>
+  <si>
+    <t>Littlefuse</t>
+  </si>
+  <si>
+    <t>0251005.NRT1L</t>
+  </si>
+  <si>
+    <t>F5566CT-ND</t>
   </si>
 </sst>
 </file>
@@ -1530,8 +1545,8 @@
   </sheetPr>
   <dimension ref="A2:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:XFD81"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1547,7 +1562,7 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2"/>
@@ -1954,7 +1969,7 @@
         <v>83</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -2000,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>90</v>
@@ -2009,16 +2024,16 @@
         <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>350</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>351</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" t="s">
-        <v>95</v>
+        <v>10</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2026,25 +2041,25 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2052,25 +2067,25 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
         <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2078,25 +2093,25 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E23" t="s">
         <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
         <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2104,25 +2119,25 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="E24" t="s">
         <v>45</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2130,25 +2145,25 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="E25" t="s">
         <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G25" t="s">
         <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2156,30 +2171,30 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="E26" t="s">
         <v>45</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28"/>
@@ -2215,25 +2230,25 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D30" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2241,25 +2256,25 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>349</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H31" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2267,25 +2282,25 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F32" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H32" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -2293,25 +2308,25 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2319,25 +2334,25 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2345,25 +2360,25 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" t="s">
         <v>142</v>
       </c>
-      <c r="E35" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" t="s">
-        <v>146</v>
-      </c>
       <c r="G35" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H35" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2371,25 +2386,25 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D36" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F36" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H36" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2397,25 +2412,25 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D37" t="s">
+        <v>229</v>
+      </c>
+      <c r="E37" t="s">
         <v>233</v>
       </c>
-      <c r="E37" t="s">
-        <v>237</v>
-      </c>
       <c r="F37" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2423,25 +2438,25 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D38" t="s">
+        <v>228</v>
+      </c>
+      <c r="E38" t="s">
+        <v>233</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" t="s">
         <v>232</v>
-      </c>
-      <c r="E38" t="s">
-        <v>237</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2449,25 +2464,25 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" t="s">
         <v>149</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" t="s">
-        <v>147</v>
-      </c>
-      <c r="E39" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39" t="s">
-        <v>152</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2475,25 +2490,25 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D40" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E40" t="s">
+        <v>147</v>
+      </c>
+      <c r="F40" t="s">
         <v>151</v>
       </c>
-      <c r="F40" t="s">
-        <v>155</v>
-      </c>
       <c r="G40" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H40" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2501,25 +2516,25 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>175</v>
-      </c>
       <c r="D41" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" t="s">
         <v>168</v>
       </c>
-      <c r="E41" t="s">
-        <v>172</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H41" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -2527,25 +2542,25 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E42" t="s">
+        <v>168</v>
+      </c>
+      <c r="F42" t="s">
+        <v>175</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
         <v>172</v>
-      </c>
-      <c r="F42" t="s">
-        <v>179</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2553,25 +2568,25 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" t="s">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
         <v>202</v>
       </c>
-      <c r="D43" t="s">
-        <v>160</v>
-      </c>
-      <c r="E43" t="s">
-        <v>204</v>
-      </c>
-      <c r="F43" t="s">
-        <v>206</v>
-      </c>
       <c r="G43" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -2579,25 +2594,25 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E44" t="s">
+        <v>200</v>
+      </c>
+      <c r="F44" t="s">
+        <v>205</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>204</v>
-      </c>
-      <c r="F44" t="s">
-        <v>209</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -2605,25 +2620,25 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D45" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E45" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F45" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H45" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2631,25 +2646,25 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E46" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H46" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -2657,25 +2672,25 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D47" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E47" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F47" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H47" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -2683,16 +2698,16 @@
         <v>2</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
@@ -2703,25 +2718,25 @@
         <v>25</v>
       </c>
       <c r="B49" t="s">
+        <v>195</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D49" t="s">
+        <v>181</v>
+      </c>
+      <c r="E49" t="s">
+        <v>200</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D49" t="s">
-        <v>185</v>
-      </c>
-      <c r="E49" t="s">
-        <v>204</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="I49" s="6"/>
     </row>
@@ -2730,25 +2745,25 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C50" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" t="s">
+        <v>217</v>
+      </c>
+      <c r="E50" t="s">
+        <v>215</v>
+      </c>
+      <c r="F50" t="s">
         <v>216</v>
       </c>
-      <c r="D50" t="s">
-        <v>221</v>
-      </c>
-      <c r="E50" t="s">
-        <v>219</v>
-      </c>
-      <c r="F50" t="s">
-        <v>220</v>
-      </c>
       <c r="G50" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H50" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -2756,25 +2771,25 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D51" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E51" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F51" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H51" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2782,37 +2797,59 @@
         <v>1</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D52" t="s">
+        <v>219</v>
+      </c>
+      <c r="E52" t="s">
+        <v>222</v>
+      </c>
+      <c r="F52" t="s">
+        <v>221</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H52" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="E52" t="s">
-        <v>226</v>
-      </c>
-      <c r="F52" t="s">
-        <v>225</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C53" s="5"/>
-      <c r="G53" s="6"/>
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D53" t="s">
+        <v>352</v>
+      </c>
+      <c r="E53" t="s">
+        <v>355</v>
+      </c>
+      <c r="F53" t="s">
+        <v>356</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55"/>
@@ -2852,31 +2889,31 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D58" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E58" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F58" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G58" t="s">
         <v>13</v>
       </c>
       <c r="H58" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -2884,31 +2921,31 @@
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E59" t="s">
+        <v>246</v>
+      </c>
+      <c r="F59" t="s">
         <v>250</v>
       </c>
-      <c r="F59" t="s">
-        <v>254</v>
-      </c>
       <c r="G59" t="s">
         <v>13</v>
       </c>
       <c r="H59" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I59" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2916,25 +2953,25 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D60" t="s">
         <v>76</v>
       </c>
       <c r="E60" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F60" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G60" t="s">
         <v>13</v>
       </c>
       <c r="H60" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
@@ -2944,31 +2981,31 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C61" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>260</v>
-      </c>
       <c r="E61" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F61" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G61" t="s">
         <v>13</v>
       </c>
       <c r="H61" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2976,25 +3013,25 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E62" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F62" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G62" t="s">
         <v>13</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
@@ -3004,25 +3041,25 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E63" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F63" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G63" t="s">
         <v>13</v>
       </c>
       <c r="H63" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
@@ -3032,25 +3069,25 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E64" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F64" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G64" t="s">
         <v>13</v>
       </c>
       <c r="H64" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="I64" s="13"/>
       <c r="J64" s="13"/>
@@ -3060,25 +3097,25 @@
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C65" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D65" t="s">
+        <v>262</v>
+      </c>
+      <c r="E65" t="s">
+        <v>246</v>
+      </c>
+      <c r="F65" t="s">
+        <v>264</v>
+      </c>
+      <c r="G65" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" t="s">
         <v>265</v>
-      </c>
-      <c r="D65" t="s">
-        <v>266</v>
-      </c>
-      <c r="E65" t="s">
-        <v>250</v>
-      </c>
-      <c r="F65" t="s">
-        <v>268</v>
-      </c>
-      <c r="G65" t="s">
-        <v>13</v>
-      </c>
-      <c r="H65" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -3086,28 +3123,28 @@
         <v>1</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>91</v>
       </c>
       <c r="E66" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G66" t="s">
         <v>13</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I66" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -3115,25 +3152,25 @@
         <v>2</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D67" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E67" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F67" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G67" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -3141,25 +3178,25 @@
         <v>1</v>
       </c>
       <c r="B68" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C68" t="s">
         <v>294</v>
       </c>
-      <c r="C68" t="s">
-        <v>298</v>
-      </c>
       <c r="D68" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E68" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F68" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G68" t="s">
         <v>13</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -3167,25 +3204,25 @@
         <v>1</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D69" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F69" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -3193,28 +3230,28 @@
         <v>1</v>
       </c>
       <c r="B70" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D70" t="s">
+        <v>303</v>
+      </c>
+      <c r="E70" t="s">
         <v>301</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D70" t="s">
-        <v>307</v>
-      </c>
-      <c r="E70" t="s">
-        <v>305</v>
-      </c>
       <c r="F70" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G70" t="s">
         <v>13</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -3222,25 +3259,25 @@
         <v>1</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D71" t="s">
+        <v>303</v>
+      </c>
+      <c r="E71" t="s">
+        <v>306</v>
+      </c>
+      <c r="F71" t="s">
         <v>307</v>
       </c>
-      <c r="E71" t="s">
-        <v>310</v>
-      </c>
-      <c r="F71" t="s">
-        <v>311</v>
-      </c>
       <c r="G71" t="s">
         <v>13</v>
       </c>
       <c r="H71" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -3248,25 +3285,25 @@
         <v>1</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D72" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E72" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G72" t="s">
         <v>13</v>
       </c>
       <c r="H72" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -3274,25 +3311,25 @@
         <v>2</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D73" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E73" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G73" t="s">
         <v>13</v>
       </c>
       <c r="H73" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -3300,28 +3337,28 @@
         <v>2</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D74" t="s">
+        <v>320</v>
+      </c>
+      <c r="E74" t="s">
+        <v>322</v>
+      </c>
+      <c r="F74" t="s">
         <v>324</v>
       </c>
-      <c r="E74" t="s">
-        <v>326</v>
-      </c>
-      <c r="F74" t="s">
-        <v>328</v>
-      </c>
       <c r="G74" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -3329,25 +3366,25 @@
         <v>1</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D75" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E75" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G75" t="s">
         <v>13</v>
       </c>
       <c r="H75" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -3355,25 +3392,25 @@
         <v>1</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D76" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E76" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F76" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G76" t="s">
         <v>13</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -3381,25 +3418,25 @@
         <v>2</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D77" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E77" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G77" t="s">
         <v>13</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -3407,25 +3444,25 @@
         <v>2</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D78" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E78" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F78" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G78" t="s">
         <v>13</v>
       </c>
       <c r="H78" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>